<commit_message>
A few fixes to the reader system unit test classes.
</commit_message>
<xml_diff>
--- a/testdata/test.xlsx
+++ b/testdata/test.xlsx
@@ -5,19 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="188" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="188" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="2ndsheet" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="2 of 3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>header1</t>
   </si>
@@ -67,13 +67,13 @@
     <t>data5</t>
   </si>
   <si>
-    <t>row with a boolean</t>
+    <t>row with a boolean formula</t>
   </si>
   <si>
     <t>data6</t>
   </si>
   <si>
-    <t>row with a formula</t>
+    <t>row with formulas</t>
   </si>
   <si>
     <t>data7</t>
@@ -116,6 +116,39 @@
   </si>
   <si>
     <t>data 2,3</t>
+  </si>
+  <si>
+    <t>a sheet</t>
+  </si>
+  <si>
+    <t>with</t>
+  </si>
+  <si>
+    <t>columns</t>
+  </si>
+  <si>
+    <t>row 1,col 1</t>
+  </si>
+  <si>
+    <t>row 1,col 2</t>
+  </si>
+  <si>
+    <t>row 1,col 3</t>
+  </si>
+  <si>
+    <t>row 1,col 4</t>
+  </si>
+  <si>
+    <t>row 2,col 1</t>
+  </si>
+  <si>
+    <t>row 2,col 2</t>
+  </si>
+  <si>
+    <t>row 2,col 3</t>
+  </si>
+  <si>
+    <t>row 2,col 4</t>
   </si>
 </sst>
 </file>
@@ -127,7 +160,7 @@
     <numFmt formatCode="MM/DD/YY" numFmtId="165"/>
     <numFmt formatCode="MM/DD/YYYY\ HH:MM:SS" numFmtId="166"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -152,6 +185,12 @@
     <font>
       <name val="Arial"/>
       <charset val="1"/>
+      <family val="2"/>
+      <b val="true"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="10"/>
@@ -199,11 +238,13 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -223,19 +264,19 @@
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A10" activeCellId="0" pane="topLeft" sqref="A10"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B9" activeCellId="0" pane="topLeft" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.7843137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.1647058823529"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.7843137254902"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.043137254902"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.7843137254902"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.9019607843137"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.4352941176471"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.9019607843137"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.243137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.9019607843137"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -249,7 +290,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -260,7 +301,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -271,7 +312,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
         <v>10</v>
       </c>
@@ -282,7 +323,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
         <v>13</v>
       </c>
@@ -296,7 +337,7 @@
         <v>256</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
         <v>15</v>
       </c>
@@ -308,19 +349,23 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="0" t="n">
-        <f aca="false">AVERAGE(2,4,8,16,32,64,128)</f>
-        <v>36.2857142857143</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
+      <c r="C8" s="2" t="n">
+        <f aca="false">AVERAGE(2,4,8,16,32,64)</f>
+        <v>21</v>
+      </c>
+      <c r="D8" s="2" t="str">
+        <f aca="false">CONCATENATE("string ","cat")</f>
+        <v>string cat</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
         <v>19</v>
       </c>
@@ -331,17 +376,17 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="2" t="n">
+      <c r="C10" s="3" t="n">
         <v>40909</v>
       </c>
-      <c r="D10" s="3" t="n">
+      <c r="D10" s="4" t="n">
         <v>40953.0930555556</v>
       </c>
     </row>
@@ -368,10 +413,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7843137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9019607843137"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -382,7 +427,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
         <v>27</v>
       </c>
@@ -393,7 +438,7 @@
         <v>29</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
         <v>30</v>
       </c>
@@ -420,16 +465,59 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C16" activeCellId="0" pane="topLeft" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7843137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9019607843137"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="1">
+      <c r="A1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="2">
+      <c r="A2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="3">
+      <c r="A3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>

</xml_diff>